<commit_message>
Few Bugs solved, and new Kpis Added.
Still Bug in Total Orders, B2B order and B2C order
</commit_message>
<xml_diff>
--- a/Requirments/kpis (1).xlsx
+++ b/Requirments/kpis (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kilianmayer/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fiverr\Current\69. magnus_myr + Killian\ForHumans\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BFB4CE-43F4-9142-8BB9-7E8A073D4F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B873316-B240-4559-8614-703F0EAD4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="138">
   <si>
     <t>KPIs</t>
   </si>
@@ -444,13 +442,19 @@
   </si>
   <si>
     <t>% YoY change (Q1 23 vs Q1 24)</t>
+  </si>
+  <si>
+    <t>Total B2B item sold</t>
+  </si>
+  <si>
+    <t>Total B2C item sold</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -470,7 +474,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,6 +499,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -513,7 +523,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -551,6 +561,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1711,18 +1724,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABD9E7-4F42-8D40-95F2-1F2838F282AB}">
-  <dimension ref="A3:DD124"/>
+  <dimension ref="A3:DD126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" ht="56" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="52.8">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1770,740 +1783,567 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="14.1" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="14.1" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="14.1" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" ht="14.1" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" ht="14.1" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" ht="14.1" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="14.1" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>136</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="14.1" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>137</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="14.1" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" ht="14.1" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:17" ht="14.1" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="Q16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" ht="14.1" customHeight="1">
       <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" ht="14.1" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" ht="14.1" customHeight="1">
       <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" ht="14.1" customHeight="1">
       <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" ht="14.1" customHeight="1">
       <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" ht="14.1" customHeight="1">
       <c r="A25" s="5"/>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" ht="14.1" customHeight="1">
       <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" ht="14.1" customHeight="1">
       <c r="A27" s="5"/>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" ht="14.1" customHeight="1">
       <c r="A28" s="5"/>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="8" t="s">
-        <v>34</v>
-      </c>
+    <row r="29" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A30" s="5"/>
       <c r="B30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:17" ht="14.1" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="10"/>
-    </row>
-    <row r="31" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
-      <c r="B31" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:17" ht="14.1" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="14.1" customHeight="1">
       <c r="A33" s="7"/>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="14.1" customHeight="1">
       <c r="A34" s="7"/>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="14.1" customHeight="1">
       <c r="A35" s="7"/>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="14.1" customHeight="1">
       <c r="A36" s="7"/>
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="14.1" customHeight="1">
       <c r="A37" s="7"/>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="14.1" customHeight="1">
       <c r="A38" s="7"/>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="14.1" customHeight="1">
       <c r="A39" s="7"/>
       <c r="B39" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="14.1" customHeight="1">
       <c r="A40" s="7"/>
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" ht="14" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="14.1" customHeight="1">
+      <c r="A41" s="7"/>
       <c r="B41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:4" ht="14.1" customHeight="1">
+      <c r="A42" s="7"/>
+      <c r="B42" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B42" s="2" t="s">
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B43" s="2" t="s">
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B44" s="2" t="s">
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B45" s="2" t="s">
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D45" s="10"/>
-    </row>
-    <row r="46" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B46" s="2" t="s">
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B47" s="2" t="s">
+    <row r="49" spans="2:3">
+      <c r="B49" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B48" s="2" t="s">
+    <row r="50" spans="2:3">
+      <c r="B50" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B49" s="2" t="s">
+    <row r="51" spans="2:3">
+      <c r="B51" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B50" s="2" t="s">
+    <row r="52" spans="2:3">
+      <c r="B52" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B51" s="2" t="s">
+    <row r="53" spans="2:3">
+      <c r="B53" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B52" s="2" t="s">
+    <row r="54" spans="2:3">
+      <c r="B54" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B53" s="2" t="s">
+    <row r="55" spans="2:3">
+      <c r="B55" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B54" s="2" t="s">
+    <row r="56" spans="2:3">
+      <c r="B56" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B55" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B56" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="2:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:3">
       <c r="B57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3">
+      <c r="B58" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B58" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B59" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="B60" s="11" t="s">
+    <row r="60" spans="2:3">
+      <c r="B60" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3">
+      <c r="B61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="39.6">
+      <c r="B62" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="2:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="B61" s="11" t="s">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="2:3" ht="26.4">
+      <c r="B63" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B62" s="11" t="s">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="2:3" ht="26.4">
+      <c r="B64" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="2:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="B63" s="11" t="s">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="2:108" ht="26.4">
+      <c r="B65" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="2:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="B64" s="11" t="s">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="2:108" ht="39.6">
+      <c r="B66" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="2:108" ht="70" x14ac:dyDescent="0.15">
-      <c r="B65" s="11" t="s">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="2:108" ht="66">
+      <c r="B67" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B66" s="11" t="s">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="2:108">
+      <c r="B68" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="I66" s="12"/>
-      <c r="L66" s="11"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
-      <c r="U66" s="11"/>
-      <c r="W66" s="12"/>
-      <c r="X66" s="12"/>
-      <c r="Y66" s="12"/>
-      <c r="Z66" s="12"/>
-      <c r="AA66" s="12"/>
-      <c r="AB66" s="12"/>
-      <c r="AC66" s="12"/>
-      <c r="AD66" s="12"/>
-      <c r="AE66" s="12"/>
-      <c r="AG66" s="12"/>
-      <c r="AI66" s="12"/>
-      <c r="AJ66" s="12"/>
-      <c r="AK66" s="12"/>
-      <c r="AL66" s="12"/>
-      <c r="AM66" s="12"/>
-      <c r="AN66" s="12"/>
-      <c r="AO66" s="12"/>
-      <c r="AP66" s="12"/>
-      <c r="AQ66" s="12"/>
-      <c r="AR66" s="12"/>
-      <c r="AS66" s="12"/>
-      <c r="AT66" s="12"/>
-      <c r="AU66" s="12"/>
-      <c r="AV66" s="12"/>
-      <c r="AX66" s="12"/>
-      <c r="AY66" s="12"/>
-      <c r="AZ66" s="12"/>
-      <c r="BA66" s="12"/>
-      <c r="BC66" s="12"/>
-      <c r="BE66" s="12"/>
-      <c r="BF66" s="12"/>
-      <c r="BG66" s="12"/>
-      <c r="BH66" s="12"/>
-      <c r="BI66" s="12"/>
-      <c r="BJ66" s="12"/>
-      <c r="BK66" s="12"/>
-      <c r="BL66" s="12"/>
-      <c r="BM66" s="12"/>
-      <c r="BN66" s="12"/>
-      <c r="BO66" s="12"/>
-      <c r="BP66" s="12"/>
-      <c r="BQ66" s="12"/>
-      <c r="BR66" s="12"/>
-      <c r="BS66" s="12"/>
-      <c r="BT66" s="12"/>
-      <c r="BU66" s="12"/>
-      <c r="BV66" s="12"/>
-      <c r="BW66" s="12"/>
-      <c r="BX66" s="12"/>
-      <c r="BY66" s="12"/>
-      <c r="BZ66" s="12"/>
-      <c r="CA66" s="12"/>
-      <c r="CB66" s="12"/>
-      <c r="CC66" s="12"/>
-      <c r="CD66" s="12"/>
-      <c r="CE66" s="12"/>
-      <c r="CF66" s="12"/>
-      <c r="CG66" s="12"/>
-      <c r="CH66" s="12"/>
-      <c r="CI66" s="12"/>
-      <c r="CJ66" s="12"/>
-      <c r="CK66" s="12"/>
-      <c r="CL66" s="12"/>
-      <c r="CM66" s="12"/>
-      <c r="CN66" s="12"/>
-      <c r="CO66" s="12"/>
-      <c r="CP66" s="12"/>
-      <c r="CQ66" s="12"/>
-      <c r="CR66" s="12"/>
-      <c r="CS66" s="12"/>
-      <c r="CT66" s="12"/>
-      <c r="CU66" s="12"/>
-      <c r="CV66" s="12"/>
-      <c r="CW66" s="12"/>
-      <c r="CX66" s="12"/>
-      <c r="CY66" s="12"/>
-      <c r="CZ66" s="12"/>
-      <c r="DA66" s="12"/>
-      <c r="DB66" s="12"/>
-      <c r="DC66" s="12"/>
-      <c r="DD66" s="12"/>
-    </row>
-    <row r="67" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B67" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="I67" s="12"/>
-      <c r="L67" s="11"/>
-      <c r="Q67" s="12"/>
-      <c r="S67" s="12"/>
-      <c r="T67" s="12"/>
-      <c r="U67" s="12"/>
-      <c r="W67" s="12"/>
-      <c r="X67" s="12"/>
-      <c r="Y67" s="12"/>
-      <c r="Z67" s="12"/>
-      <c r="AA67" s="12"/>
-      <c r="AB67" s="12"/>
-      <c r="AC67" s="12"/>
-      <c r="AD67" s="12"/>
-      <c r="AE67" s="12"/>
-      <c r="AG67" s="12"/>
-      <c r="AH67" s="12"/>
-      <c r="AI67" s="12"/>
-      <c r="AJ67" s="12"/>
-      <c r="AK67" s="12"/>
-      <c r="AL67" s="12"/>
-      <c r="AM67" s="12"/>
-      <c r="AN67" s="12"/>
-      <c r="AO67" s="12"/>
-      <c r="AP67" s="12"/>
-      <c r="AQ67" s="12"/>
-      <c r="AR67" s="12"/>
-      <c r="AS67" s="12"/>
-      <c r="AT67" s="12"/>
-      <c r="AU67" s="12"/>
-      <c r="AV67" s="12"/>
-      <c r="AW67" s="12"/>
-      <c r="AX67" s="12"/>
-      <c r="AY67" s="12"/>
-      <c r="AZ67" s="12"/>
-      <c r="BA67" s="12"/>
-      <c r="BC67" s="12"/>
-      <c r="BE67" s="12"/>
-      <c r="BF67" s="12"/>
-      <c r="BG67" s="12"/>
-      <c r="BH67" s="12"/>
-      <c r="BI67" s="12"/>
-      <c r="BJ67" s="12"/>
-      <c r="BK67" s="12"/>
-      <c r="BL67" s="12"/>
-      <c r="BM67" s="12"/>
-      <c r="BN67" s="12"/>
-      <c r="BO67" s="12"/>
-      <c r="BP67" s="12"/>
-      <c r="BQ67" s="12"/>
-      <c r="BR67" s="12"/>
-      <c r="BS67" s="12"/>
-      <c r="BT67" s="12"/>
-      <c r="BU67" s="12"/>
-      <c r="BV67" s="12"/>
-      <c r="BW67" s="12"/>
-      <c r="BX67" s="12"/>
-      <c r="BY67" s="12"/>
-      <c r="BZ67" s="12"/>
-      <c r="CA67" s="12"/>
-      <c r="CB67" s="12"/>
-      <c r="CC67" s="12"/>
-      <c r="CD67" s="12"/>
-      <c r="CE67" s="12"/>
-      <c r="CF67" s="12"/>
-      <c r="CG67" s="12"/>
-      <c r="CH67" s="12"/>
-      <c r="CI67" s="12"/>
-      <c r="CJ67" s="12"/>
-      <c r="CK67" s="12"/>
-      <c r="CL67" s="12"/>
-      <c r="CM67" s="12"/>
-      <c r="CN67" s="12"/>
-      <c r="CO67" s="12"/>
-      <c r="CP67" s="12"/>
-      <c r="CQ67" s="12"/>
-      <c r="CR67" s="12"/>
-      <c r="CS67" s="12"/>
-      <c r="CT67" s="12"/>
-      <c r="CU67" s="12"/>
-      <c r="CV67" s="12"/>
-      <c r="CW67" s="12"/>
-      <c r="CX67" s="12"/>
-      <c r="CY67" s="12"/>
-      <c r="CZ67" s="12"/>
-      <c r="DA67" s="12"/>
-      <c r="DB67" s="12"/>
-      <c r="DC67" s="12"/>
-      <c r="DD67" s="12"/>
-    </row>
-    <row r="68" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B68" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
@@ -2511,12 +2351,9 @@
       <c r="G68" s="11"/>
       <c r="I68" s="12"/>
       <c r="L68" s="11"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12"/>
-      <c r="Q68" s="12"/>
-      <c r="S68" s="12"/>
-      <c r="T68" s="12"/>
-      <c r="U68" s="12"/>
+      <c r="S68" s="11"/>
+      <c r="T68" s="11"/>
+      <c r="U68" s="11"/>
       <c r="W68" s="12"/>
       <c r="X68" s="12"/>
       <c r="Y68" s="12"/>
@@ -2527,7 +2364,6 @@
       <c r="AD68" s="12"/>
       <c r="AE68" s="12"/>
       <c r="AG68" s="12"/>
-      <c r="AH68" s="12"/>
       <c r="AI68" s="12"/>
       <c r="AJ68" s="12"/>
       <c r="AK68" s="12"/>
@@ -2542,7 +2378,6 @@
       <c r="AT68" s="12"/>
       <c r="AU68" s="12"/>
       <c r="AV68" s="12"/>
-      <c r="AW68" s="12"/>
       <c r="AX68" s="12"/>
       <c r="AY68" s="12"/>
       <c r="AZ68" s="12"/>
@@ -2601,228 +2436,215 @@
       <c r="DC68" s="12"/>
       <c r="DD68" s="12"/>
     </row>
-    <row r="69" spans="2:108" ht="14" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:108">
       <c r="B69" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="I69" s="12"/>
+      <c r="L69" s="11"/>
+      <c r="Q69" s="12"/>
+      <c r="S69" s="12"/>
+      <c r="T69" s="12"/>
+      <c r="U69" s="12"/>
+      <c r="W69" s="12"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+      <c r="AA69" s="12"/>
+      <c r="AB69" s="12"/>
+      <c r="AC69" s="12"/>
+      <c r="AD69" s="12"/>
+      <c r="AE69" s="12"/>
+      <c r="AG69" s="12"/>
+      <c r="AH69" s="12"/>
+      <c r="AI69" s="12"/>
+      <c r="AJ69" s="12"/>
+      <c r="AK69" s="12"/>
+      <c r="AL69" s="12"/>
+      <c r="AM69" s="12"/>
+      <c r="AN69" s="12"/>
+      <c r="AO69" s="12"/>
+      <c r="AP69" s="12"/>
+      <c r="AQ69" s="12"/>
+      <c r="AR69" s="12"/>
+      <c r="AS69" s="12"/>
+      <c r="AT69" s="12"/>
+      <c r="AU69" s="12"/>
+      <c r="AV69" s="12"/>
+      <c r="AW69" s="12"/>
+      <c r="AX69" s="12"/>
+      <c r="AY69" s="12"/>
+      <c r="AZ69" s="12"/>
+      <c r="BA69" s="12"/>
+      <c r="BC69" s="12"/>
+      <c r="BE69" s="12"/>
+      <c r="BF69" s="12"/>
+      <c r="BG69" s="12"/>
+      <c r="BH69" s="12"/>
+      <c r="BI69" s="12"/>
+      <c r="BJ69" s="12"/>
+      <c r="BK69" s="12"/>
+      <c r="BL69" s="12"/>
+      <c r="BM69" s="12"/>
+      <c r="BN69" s="12"/>
+      <c r="BO69" s="12"/>
+      <c r="BP69" s="12"/>
+      <c r="BQ69" s="12"/>
+      <c r="BR69" s="12"/>
+      <c r="BS69" s="12"/>
+      <c r="BT69" s="12"/>
+      <c r="BU69" s="12"/>
+      <c r="BV69" s="12"/>
+      <c r="BW69" s="12"/>
+      <c r="BX69" s="12"/>
+      <c r="BY69" s="12"/>
+      <c r="BZ69" s="12"/>
+      <c r="CA69" s="12"/>
+      <c r="CB69" s="12"/>
+      <c r="CC69" s="12"/>
+      <c r="CD69" s="12"/>
+      <c r="CE69" s="12"/>
+      <c r="CF69" s="12"/>
+      <c r="CG69" s="12"/>
+      <c r="CH69" s="12"/>
+      <c r="CI69" s="12"/>
+      <c r="CJ69" s="12"/>
+      <c r="CK69" s="12"/>
+      <c r="CL69" s="12"/>
+      <c r="CM69" s="12"/>
+      <c r="CN69" s="12"/>
+      <c r="CO69" s="12"/>
+      <c r="CP69" s="12"/>
+      <c r="CQ69" s="12"/>
+      <c r="CR69" s="12"/>
+      <c r="CS69" s="12"/>
+      <c r="CT69" s="12"/>
+      <c r="CU69" s="12"/>
+      <c r="CV69" s="12"/>
+      <c r="CW69" s="12"/>
+      <c r="CX69" s="12"/>
+      <c r="CY69" s="12"/>
+      <c r="CZ69" s="12"/>
+      <c r="DA69" s="12"/>
+      <c r="DB69" s="12"/>
+      <c r="DC69" s="12"/>
+      <c r="DD69" s="12"/>
+    </row>
+    <row r="70" spans="2:108">
+      <c r="B70" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="I70" s="12"/>
+      <c r="L70" s="11"/>
+      <c r="N70" s="12"/>
+      <c r="O70" s="12"/>
+      <c r="Q70" s="12"/>
+      <c r="S70" s="12"/>
+      <c r="T70" s="12"/>
+      <c r="U70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="12"/>
+      <c r="AC70" s="12"/>
+      <c r="AD70" s="12"/>
+      <c r="AE70" s="12"/>
+      <c r="AG70" s="12"/>
+      <c r="AH70" s="12"/>
+      <c r="AI70" s="12"/>
+      <c r="AJ70" s="12"/>
+      <c r="AK70" s="12"/>
+      <c r="AL70" s="12"/>
+      <c r="AM70" s="12"/>
+      <c r="AN70" s="12"/>
+      <c r="AO70" s="12"/>
+      <c r="AP70" s="12"/>
+      <c r="AQ70" s="12"/>
+      <c r="AR70" s="12"/>
+      <c r="AS70" s="12"/>
+      <c r="AT70" s="12"/>
+      <c r="AU70" s="12"/>
+      <c r="AV70" s="12"/>
+      <c r="AW70" s="12"/>
+      <c r="AX70" s="12"/>
+      <c r="AY70" s="12"/>
+      <c r="AZ70" s="12"/>
+      <c r="BA70" s="12"/>
+      <c r="BC70" s="12"/>
+      <c r="BE70" s="12"/>
+      <c r="BF70" s="12"/>
+      <c r="BG70" s="12"/>
+      <c r="BH70" s="12"/>
+      <c r="BI70" s="12"/>
+      <c r="BJ70" s="12"/>
+      <c r="BK70" s="12"/>
+      <c r="BL70" s="12"/>
+      <c r="BM70" s="12"/>
+      <c r="BN70" s="12"/>
+      <c r="BO70" s="12"/>
+      <c r="BP70" s="12"/>
+      <c r="BQ70" s="12"/>
+      <c r="BR70" s="12"/>
+      <c r="BS70" s="12"/>
+      <c r="BT70" s="12"/>
+      <c r="BU70" s="12"/>
+      <c r="BV70" s="12"/>
+      <c r="BW70" s="12"/>
+      <c r="BX70" s="12"/>
+      <c r="BY70" s="12"/>
+      <c r="BZ70" s="12"/>
+      <c r="CA70" s="12"/>
+      <c r="CB70" s="12"/>
+      <c r="CC70" s="12"/>
+      <c r="CD70" s="12"/>
+      <c r="CE70" s="12"/>
+      <c r="CF70" s="12"/>
+      <c r="CG70" s="12"/>
+      <c r="CH70" s="12"/>
+      <c r="CI70" s="12"/>
+      <c r="CJ70" s="12"/>
+      <c r="CK70" s="12"/>
+      <c r="CL70" s="12"/>
+      <c r="CM70" s="12"/>
+      <c r="CN70" s="12"/>
+      <c r="CO70" s="12"/>
+      <c r="CP70" s="12"/>
+      <c r="CQ70" s="12"/>
+      <c r="CR70" s="12"/>
+      <c r="CS70" s="12"/>
+      <c r="CT70" s="12"/>
+      <c r="CU70" s="12"/>
+      <c r="CV70" s="12"/>
+      <c r="CW70" s="12"/>
+      <c r="CX70" s="12"/>
+      <c r="CY70" s="12"/>
+      <c r="CZ70" s="12"/>
+      <c r="DA70" s="12"/>
+      <c r="DB70" s="12"/>
+      <c r="DC70" s="12"/>
+      <c r="DD70" s="12"/>
+    </row>
+    <row r="71" spans="2:108">
+      <c r="B71" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="11"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="L69" s="11"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="W69" s="1"/>
-      <c r="X69" s="1"/>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="1"/>
-      <c r="AA69" s="1"/>
-      <c r="AB69" s="1"/>
-      <c r="AC69" s="1"/>
-      <c r="AD69" s="1"/>
-      <c r="AE69" s="1"/>
-      <c r="AF69" s="1"/>
-      <c r="AG69" s="1"/>
-      <c r="AH69" s="1"/>
-      <c r="AI69" s="1"/>
-      <c r="AJ69" s="1"/>
-      <c r="AK69" s="1"/>
-      <c r="AL69" s="1"/>
-      <c r="AM69" s="1"/>
-      <c r="AN69" s="1"/>
-      <c r="AO69" s="1"/>
-      <c r="AP69" s="1"/>
-      <c r="AQ69" s="1"/>
-      <c r="AR69" s="1"/>
-      <c r="AS69" s="1"/>
-      <c r="AT69" s="1"/>
-      <c r="AU69" s="1"/>
-      <c r="AV69" s="1"/>
-      <c r="AW69" s="1"/>
-      <c r="AX69" s="1"/>
-      <c r="AY69" s="1"/>
-      <c r="AZ69" s="1"/>
-      <c r="BA69" s="1"/>
-      <c r="BC69" s="1"/>
-      <c r="BE69" s="1"/>
-      <c r="BF69" s="1"/>
-      <c r="BG69" s="1"/>
-      <c r="BH69" s="1"/>
-      <c r="BI69" s="1"/>
-      <c r="BJ69" s="1"/>
-      <c r="BK69" s="1"/>
-      <c r="BL69" s="1"/>
-      <c r="BM69" s="1"/>
-      <c r="BN69" s="1"/>
-      <c r="BO69" s="1"/>
-      <c r="BP69" s="1"/>
-      <c r="BQ69" s="1"/>
-      <c r="BR69" s="1"/>
-      <c r="BS69" s="1"/>
-      <c r="BT69" s="1"/>
-      <c r="BU69" s="1"/>
-      <c r="BV69" s="1"/>
-      <c r="BW69" s="1"/>
-      <c r="BX69" s="1"/>
-      <c r="BY69" s="1"/>
-      <c r="BZ69" s="1"/>
-      <c r="CA69" s="1"/>
-      <c r="CB69" s="1"/>
-      <c r="CC69" s="1"/>
-      <c r="CD69" s="1"/>
-      <c r="CE69" s="1"/>
-      <c r="CF69" s="1"/>
-      <c r="CG69" s="1"/>
-      <c r="CH69" s="1"/>
-      <c r="CI69" s="1"/>
-      <c r="CJ69" s="1"/>
-      <c r="CK69" s="1"/>
-      <c r="CL69" s="1"/>
-      <c r="CM69" s="1"/>
-      <c r="CN69" s="1"/>
-      <c r="CO69" s="1"/>
-      <c r="CP69" s="1"/>
-      <c r="CQ69" s="1"/>
-      <c r="CR69" s="1"/>
-      <c r="CS69" s="1"/>
-      <c r="CT69" s="1"/>
-      <c r="CU69" s="1"/>
-      <c r="CV69" s="1"/>
-      <c r="CW69" s="1"/>
-      <c r="CX69" s="1"/>
-      <c r="CY69" s="1"/>
-      <c r="CZ69" s="1"/>
-      <c r="DA69" s="1"/>
-      <c r="DB69" s="1"/>
-      <c r="DC69" s="1"/>
-      <c r="DD69" s="1"/>
-    </row>
-    <row r="70" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B70" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="W70" s="1"/>
-      <c r="X70" s="1"/>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="1"/>
-      <c r="AA70" s="1"/>
-      <c r="AB70" s="1"/>
-      <c r="AC70" s="1"/>
-      <c r="AD70" s="1"/>
-      <c r="AE70" s="1"/>
-      <c r="AF70" s="1"/>
-      <c r="AG70" s="1"/>
-      <c r="AH70" s="1"/>
-      <c r="AI70" s="1"/>
-      <c r="AJ70" s="1"/>
-      <c r="AK70" s="1"/>
-      <c r="AL70" s="1"/>
-      <c r="AM70" s="1"/>
-      <c r="AN70" s="1"/>
-      <c r="AO70" s="1"/>
-      <c r="AP70" s="1"/>
-      <c r="AQ70" s="1"/>
-      <c r="AR70" s="1"/>
-      <c r="AS70" s="1"/>
-      <c r="AT70" s="1"/>
-      <c r="AU70" s="1"/>
-      <c r="AV70" s="1"/>
-      <c r="AW70" s="1"/>
-      <c r="AX70" s="1"/>
-      <c r="AY70" s="1"/>
-      <c r="AZ70" s="1"/>
-      <c r="BA70" s="1"/>
-      <c r="BC70" s="1"/>
-      <c r="BE70" s="1"/>
-      <c r="BF70" s="1"/>
-      <c r="BG70" s="1"/>
-      <c r="BH70" s="1"/>
-      <c r="BI70" s="1"/>
-      <c r="BJ70" s="1"/>
-      <c r="BK70" s="1"/>
-      <c r="BL70" s="1"/>
-      <c r="BM70" s="1"/>
-      <c r="BN70" s="1"/>
-      <c r="BO70" s="1"/>
-      <c r="BP70" s="1"/>
-      <c r="BQ70" s="1"/>
-      <c r="BR70" s="1"/>
-      <c r="BS70" s="1"/>
-      <c r="BT70" s="1"/>
-      <c r="BU70" s="1"/>
-      <c r="BV70" s="1"/>
-      <c r="BW70" s="1"/>
-      <c r="BX70" s="1"/>
-      <c r="BY70" s="1"/>
-      <c r="BZ70" s="1"/>
-      <c r="CA70" s="1"/>
-      <c r="CB70" s="1"/>
-      <c r="CC70" s="1"/>
-      <c r="CD70" s="1"/>
-      <c r="CE70" s="1"/>
-      <c r="CF70" s="1"/>
-      <c r="CG70" s="1"/>
-      <c r="CH70" s="1"/>
-      <c r="CI70" s="1"/>
-      <c r="CJ70" s="1"/>
-      <c r="CK70" s="1"/>
-      <c r="CL70" s="1"/>
-      <c r="CM70" s="1"/>
-      <c r="CN70" s="1"/>
-      <c r="CO70" s="1"/>
-      <c r="CP70" s="1"/>
-      <c r="CQ70" s="1"/>
-      <c r="CR70" s="1"/>
-      <c r="CS70" s="1"/>
-      <c r="CT70" s="1"/>
-      <c r="CU70" s="1"/>
-      <c r="CV70" s="1"/>
-      <c r="CW70" s="1"/>
-      <c r="CX70" s="1"/>
-      <c r="CY70" s="1"/>
-      <c r="CZ70" s="1"/>
-      <c r="DA70" s="1"/>
-      <c r="DB70" s="1"/>
-      <c r="DC70" s="1"/>
-      <c r="DD70" s="1"/>
-    </row>
-    <row r="71" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B71" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-      <c r="J71" s="11"/>
       <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="Q71" s="1"/>
@@ -2915,11 +2737,10 @@
       <c r="DC71" s="1"/>
       <c r="DD71" s="1"/>
     </row>
-    <row r="72" spans="2:108" ht="28" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:108">
       <c r="B72" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C72" s="11"/>
+        <v>114</v>
+      </c>
       <c r="D72" s="11"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -2931,13 +2752,11 @@
       <c r="M72" s="11"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
-      <c r="V72" s="1"/>
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
       <c r="Y72" s="1"/>
@@ -2970,7 +2789,6 @@
       <c r="AZ72" s="1"/>
       <c r="BA72" s="1"/>
       <c r="BC72" s="1"/>
-      <c r="BD72" s="1"/>
       <c r="BE72" s="1"/>
       <c r="BF72" s="1"/>
       <c r="BG72" s="1"/>
@@ -3024,263 +2842,478 @@
       <c r="DC72" s="1"/>
       <c r="DD72" s="1"/>
     </row>
-    <row r="73" spans="2:108" ht="28" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:108">
       <c r="B73" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="11"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AB73" s="1"/>
+      <c r="AC73" s="1"/>
+      <c r="AD73" s="1"/>
+      <c r="AE73" s="1"/>
+      <c r="AF73" s="1"/>
+      <c r="AG73" s="1"/>
+      <c r="AH73" s="1"/>
+      <c r="AI73" s="1"/>
+      <c r="AJ73" s="1"/>
+      <c r="AK73" s="1"/>
+      <c r="AL73" s="1"/>
+      <c r="AM73" s="1"/>
+      <c r="AN73" s="1"/>
+      <c r="AO73" s="1"/>
+      <c r="AP73" s="1"/>
+      <c r="AQ73" s="1"/>
+      <c r="AR73" s="1"/>
+      <c r="AS73" s="1"/>
+      <c r="AT73" s="1"/>
+      <c r="AU73" s="1"/>
+      <c r="AV73" s="1"/>
+      <c r="AW73" s="1"/>
+      <c r="AX73" s="1"/>
+      <c r="AY73" s="1"/>
+      <c r="AZ73" s="1"/>
+      <c r="BA73" s="1"/>
+      <c r="BC73" s="1"/>
+      <c r="BE73" s="1"/>
+      <c r="BF73" s="1"/>
+      <c r="BG73" s="1"/>
+      <c r="BH73" s="1"/>
+      <c r="BI73" s="1"/>
+      <c r="BJ73" s="1"/>
+      <c r="BK73" s="1"/>
+      <c r="BL73" s="1"/>
+      <c r="BM73" s="1"/>
+      <c r="BN73" s="1"/>
+      <c r="BO73" s="1"/>
+      <c r="BP73" s="1"/>
+      <c r="BQ73" s="1"/>
+      <c r="BR73" s="1"/>
+      <c r="BS73" s="1"/>
+      <c r="BT73" s="1"/>
+      <c r="BU73" s="1"/>
+      <c r="BV73" s="1"/>
+      <c r="BW73" s="1"/>
+      <c r="BX73" s="1"/>
+      <c r="BY73" s="1"/>
+      <c r="BZ73" s="1"/>
+      <c r="CA73" s="1"/>
+      <c r="CB73" s="1"/>
+      <c r="CC73" s="1"/>
+      <c r="CD73" s="1"/>
+      <c r="CE73" s="1"/>
+      <c r="CF73" s="1"/>
+      <c r="CG73" s="1"/>
+      <c r="CH73" s="1"/>
+      <c r="CI73" s="1"/>
+      <c r="CJ73" s="1"/>
+      <c r="CK73" s="1"/>
+      <c r="CL73" s="1"/>
+      <c r="CM73" s="1"/>
+      <c r="CN73" s="1"/>
+      <c r="CO73" s="1"/>
+      <c r="CP73" s="1"/>
+      <c r="CQ73" s="1"/>
+      <c r="CR73" s="1"/>
+      <c r="CS73" s="1"/>
+      <c r="CT73" s="1"/>
+      <c r="CU73" s="1"/>
+      <c r="CV73" s="1"/>
+      <c r="CW73" s="1"/>
+      <c r="CX73" s="1"/>
+      <c r="CY73" s="1"/>
+      <c r="CZ73" s="1"/>
+      <c r="DA73" s="1"/>
+      <c r="DB73" s="1"/>
+      <c r="DC73" s="1"/>
+      <c r="DD73" s="1"/>
+    </row>
+    <row r="74" spans="2:108" ht="26.4">
+      <c r="B74" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="11"/>
+      <c r="L74" s="11"/>
+      <c r="M74" s="11"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
+      <c r="Z74" s="1"/>
+      <c r="AA74" s="1"/>
+      <c r="AB74" s="1"/>
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+      <c r="AF74" s="1"/>
+      <c r="AG74" s="1"/>
+      <c r="AH74" s="1"/>
+      <c r="AI74" s="1"/>
+      <c r="AJ74" s="1"/>
+      <c r="AK74" s="1"/>
+      <c r="AL74" s="1"/>
+      <c r="AM74" s="1"/>
+      <c r="AN74" s="1"/>
+      <c r="AO74" s="1"/>
+      <c r="AP74" s="1"/>
+      <c r="AQ74" s="1"/>
+      <c r="AR74" s="1"/>
+      <c r="AS74" s="1"/>
+      <c r="AT74" s="1"/>
+      <c r="AU74" s="1"/>
+      <c r="AV74" s="1"/>
+      <c r="AW74" s="1"/>
+      <c r="AX74" s="1"/>
+      <c r="AY74" s="1"/>
+      <c r="AZ74" s="1"/>
+      <c r="BA74" s="1"/>
+      <c r="BC74" s="1"/>
+      <c r="BD74" s="1"/>
+      <c r="BE74" s="1"/>
+      <c r="BF74" s="1"/>
+      <c r="BG74" s="1"/>
+      <c r="BH74" s="1"/>
+      <c r="BI74" s="1"/>
+      <c r="BJ74" s="1"/>
+      <c r="BK74" s="1"/>
+      <c r="BL74" s="1"/>
+      <c r="BM74" s="1"/>
+      <c r="BN74" s="1"/>
+      <c r="BO74" s="1"/>
+      <c r="BP74" s="1"/>
+      <c r="BQ74" s="1"/>
+      <c r="BR74" s="1"/>
+      <c r="BS74" s="1"/>
+      <c r="BT74" s="1"/>
+      <c r="BU74" s="1"/>
+      <c r="BV74" s="1"/>
+      <c r="BW74" s="1"/>
+      <c r="BX74" s="1"/>
+      <c r="BY74" s="1"/>
+      <c r="BZ74" s="1"/>
+      <c r="CA74" s="1"/>
+      <c r="CB74" s="1"/>
+      <c r="CC74" s="1"/>
+      <c r="CD74" s="1"/>
+      <c r="CE74" s="1"/>
+      <c r="CF74" s="1"/>
+      <c r="CG74" s="1"/>
+      <c r="CH74" s="1"/>
+      <c r="CI74" s="1"/>
+      <c r="CJ74" s="1"/>
+      <c r="CK74" s="1"/>
+      <c r="CL74" s="1"/>
+      <c r="CM74" s="1"/>
+      <c r="CN74" s="1"/>
+      <c r="CO74" s="1"/>
+      <c r="CP74" s="1"/>
+      <c r="CQ74" s="1"/>
+      <c r="CR74" s="1"/>
+      <c r="CS74" s="1"/>
+      <c r="CT74" s="1"/>
+      <c r="CU74" s="1"/>
+      <c r="CV74" s="1"/>
+      <c r="CW74" s="1"/>
+      <c r="CX74" s="1"/>
+      <c r="CY74" s="1"/>
+      <c r="CZ74" s="1"/>
+      <c r="DA74" s="1"/>
+      <c r="DB74" s="1"/>
+      <c r="DC74" s="1"/>
+      <c r="DD74" s="1"/>
+    </row>
+    <row r="75" spans="2:108" ht="26.4">
+      <c r="B75" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="2:108" ht="28" x14ac:dyDescent="0.15">
-      <c r="B74" s="11" t="s">
+    <row r="76" spans="2:108" ht="26.4">
+      <c r="B76" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B75" s="11" t="s">
+    <row r="77" spans="2:108">
+      <c r="B77" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B76" s="11" t="s">
+    <row r="78" spans="2:108">
+      <c r="B78" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="2:108" ht="28" x14ac:dyDescent="0.15">
-      <c r="B77" s="11" t="s">
+    <row r="79" spans="2:108" ht="26.4">
+      <c r="B79" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="2:108" ht="28" x14ac:dyDescent="0.15">
-      <c r="B78" s="11" t="s">
+    <row r="80" spans="2:108" ht="26.4">
+      <c r="B80" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="79" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B79" s="11" t="s">
+    <row r="81" spans="2:2">
+      <c r="B81" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="2:108" ht="14" x14ac:dyDescent="0.15">
-      <c r="B80" s="11" t="s">
+    <row r="82" spans="2:2">
+      <c r="B82" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B81" s="11" t="s">
+    <row r="83" spans="2:2">
+      <c r="B83" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B82" s="11" t="s">
+    <row r="84" spans="2:2" ht="26.4">
+      <c r="B84" s="11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B83" s="11" t="s">
+    <row r="85" spans="2:2" ht="26.4">
+      <c r="B85" s="11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B84" s="11" t="s">
+    <row r="86" spans="2:2" ht="26.4">
+      <c r="B86" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="85" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B85" s="11" t="s">
+    <row r="87" spans="2:2" ht="26.4">
+      <c r="B87" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B86" s="11" t="s">
+    <row r="88" spans="2:2">
+      <c r="B88" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B87" s="11" t="s">
+    <row r="89" spans="2:2">
+      <c r="B89" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B88" s="11" t="s">
+    <row r="90" spans="2:2" ht="26.4">
+      <c r="B90" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B89" s="11" t="s">
+    <row r="91" spans="2:2" ht="26.4">
+      <c r="B91" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="90" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B90" s="11" t="s">
+    <row r="92" spans="2:2" ht="26.4">
+      <c r="B92" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B91" s="11" t="s">
+    <row r="93" spans="2:2" ht="26.4">
+      <c r="B93" s="11" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B92" s="11" t="s">
+    <row r="94" spans="2:2">
+      <c r="B94" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B93" s="12" t="s">
+    <row r="95" spans="2:2" ht="26.4">
+      <c r="B95" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="94" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B94" s="11" t="s">
+    <row r="96" spans="2:2" ht="26.4">
+      <c r="B96" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B95" s="11" t="s">
+    <row r="97" spans="2:2" ht="26.4">
+      <c r="B97" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B96" s="11" t="s">
+    <row r="98" spans="2:2" ht="26.4">
+      <c r="B98" s="11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="42" x14ac:dyDescent="0.15">
-      <c r="B97" s="11" t="s">
+    <row r="99" spans="2:2" ht="39.6">
+      <c r="B99" s="11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="42" x14ac:dyDescent="0.15">
-      <c r="B98" s="11" t="s">
+    <row r="100" spans="2:2" ht="39.6">
+      <c r="B100" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B99" s="11" t="s">
+    <row r="101" spans="2:2" ht="26.4">
+      <c r="B101" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B100" s="11" t="s">
+    <row r="102" spans="2:2" ht="26.4">
+      <c r="B102" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B101" s="11" t="s">
+    <row r="103" spans="2:2">
+      <c r="B103" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B102" s="11" t="s">
+    <row r="104" spans="2:2">
+      <c r="B104" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B103" s="11" t="s">
+    <row r="105" spans="2:2">
+      <c r="B105" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B104" s="11" t="s">
+    <row r="106" spans="2:2" ht="26.4">
+      <c r="B106" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B105" s="11" t="s">
+    <row r="107" spans="2:2">
+      <c r="B107" s="11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B106" s="11" t="s">
+    <row r="108" spans="2:2">
+      <c r="B108" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="107" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B107" s="11" t="s">
+    <row r="109" spans="2:2" ht="26.4">
+      <c r="B109" s="11" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B108" s="11" t="s">
+    <row r="110" spans="2:2">
+      <c r="B110" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B109" s="11" t="s">
+    <row r="111" spans="2:2">
+      <c r="B111" s="11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="42" x14ac:dyDescent="0.15">
-      <c r="B110" s="11" t="s">
+    <row r="112" spans="2:2" ht="39.6">
+      <c r="B112" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B111" s="11" t="s">
+    <row r="113" spans="2:2" ht="39.6">
+      <c r="B113" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B112" s="11" t="s">
+    <row r="114" spans="2:2" ht="26.4">
+      <c r="B114" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B113" s="11" t="s">
+    <row r="115" spans="2:2" ht="26.4">
+      <c r="B115" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="114" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B114" s="11" t="s">
+    <row r="116" spans="2:2">
+      <c r="B116" s="11" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="115" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B115" s="11" t="s">
+    <row r="117" spans="2:2">
+      <c r="B117" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B116" s="11" t="s">
+    <row r="118" spans="2:2">
+      <c r="B118" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="117" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B117" s="11" t="s">
+    <row r="119" spans="2:2">
+      <c r="B119" s="11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B118" s="11" t="s">
+    <row r="120" spans="2:2">
+      <c r="B120" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B119" s="11" t="s">
+    <row r="121" spans="2:2">
+      <c r="B121" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="120" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B120" s="11" t="s">
+    <row r="122" spans="2:2">
+      <c r="B122" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="121" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B121" s="11" t="s">
+    <row r="123" spans="2:2">
+      <c r="B123" s="11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="122" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B122" s="11" t="s">
+    <row r="124" spans="2:2" ht="26.4">
+      <c r="B124" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B123" s="11" t="s">
+    <row r="125" spans="2:2" ht="26.4">
+      <c r="B125" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="124" spans="2:2" ht="28" x14ac:dyDescent="0.15">
-      <c r="B124" s="11" t="s">
+    <row r="126" spans="2:2" ht="26.4">
+      <c r="B126" s="11" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Few more KPIs and Bugs solved
</commit_message>
<xml_diff>
--- a/Requirments/kpis (1).xlsx
+++ b/Requirments/kpis (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fiverr\Current\69. magnus_myr + Killian\ForHumans\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B873316-B240-4559-8614-703F0EAD4F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC865F5E-7357-4124-8EE2-DAF603FD12D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="2244" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="2" r:id="rId1"/>
@@ -1726,16 +1726,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFABD9E7-4F42-8D40-95F2-1F2838F282AB}">
   <dimension ref="A3:DD126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="131" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" ht="52.8">
+    <row r="3" spans="1:17" ht="51">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1793,9 @@
       <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="14.1" customHeight="1">
       <c r="A5" s="3"/>
@@ -1803,7 +1805,9 @@
       <c r="C5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="14.1" customHeight="1">
       <c r="A6" s="3"/>
@@ -1813,7 +1817,9 @@
       <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="14.1" customHeight="1">
       <c r="A7" s="3"/>
@@ -1823,7 +1829,9 @@
       <c r="C7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="13">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="14.1" customHeight="1">
       <c r="A8" s="3"/>
@@ -1833,7 +1841,9 @@
       <c r="C8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="13">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="14.1" customHeight="1">
       <c r="A9" s="3"/>
@@ -1843,7 +1853,9 @@
       <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="13">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
@@ -1853,7 +1865,9 @@
       <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="13">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="14.1" customHeight="1">
       <c r="A11" s="3"/>
@@ -1863,7 +1877,9 @@
       <c r="C11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="13">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="14.1" customHeight="1">
       <c r="A12" s="3"/>
@@ -1873,57 +1889,69 @@
       <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="13">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="14.1" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="13">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="14.1" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="13">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="14.1" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:17" ht="14.1" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="13">
+        <v>14</v>
+      </c>
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" ht="14.1" customHeight="1">
@@ -1931,10 +1959,12 @@
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="13">
+        <v>15</v>
+      </c>
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" ht="14.1" customHeight="1">
@@ -1947,7 +1977,9 @@
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:17" ht="14.1" customHeight="1">
       <c r="A20" s="5"/>
@@ -1957,7 +1989,9 @@
       <c r="C20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:17" ht="14.1" customHeight="1">
       <c r="A21" s="5"/>
@@ -1967,7 +2001,9 @@
       <c r="C21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="14.1" customHeight="1">
       <c r="A22" s="5"/>
@@ -1977,7 +2013,9 @@
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="14.1" customHeight="1">
       <c r="A23" s="5"/>
@@ -1987,7 +2025,9 @@
       <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:17" ht="14.1" customHeight="1">
       <c r="A24" s="5"/>
@@ -1997,7 +2037,9 @@
       <c r="C24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10">
+        <v>21</v>
+      </c>
     </row>
     <row r="25" spans="1:17" ht="14.1" customHeight="1">
       <c r="A25" s="5"/>
@@ -2007,7 +2049,9 @@
       <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" spans="1:17" ht="14.1" customHeight="1">
       <c r="A26" s="5"/>
@@ -2017,7 +2061,9 @@
       <c r="C26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:17" ht="14.1" customHeight="1">
       <c r="A27" s="5"/>
@@ -2027,7 +2073,9 @@
       <c r="C27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="10">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" spans="1:17" ht="14.1" customHeight="1">
       <c r="A28" s="5"/>
@@ -2037,7 +2085,9 @@
       <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="1:17" ht="14.1" customHeight="1">
       <c r="A29" s="5"/>
@@ -2047,7 +2097,9 @@
       <c r="C29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" spans="1:17" ht="14.1" customHeight="1">
       <c r="A30" s="5"/>
@@ -2057,7 +2109,9 @@
       <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:17" ht="14.1" customHeight="1">
       <c r="A31" s="8" t="s">
@@ -2069,7 +2123,9 @@
       <c r="C31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="10"/>
+      <c r="D31" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:17" ht="14.1" customHeight="1">
       <c r="A32" s="7"/>
@@ -2079,7 +2135,9 @@
       <c r="C32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="10">
+        <v>29</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="14.1" customHeight="1">
       <c r="A33" s="7"/>
@@ -2089,7 +2147,9 @@
       <c r="C33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="14.1" customHeight="1">
       <c r="A34" s="7"/>
@@ -2099,7 +2159,9 @@
       <c r="C34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="10">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="14.1" customHeight="1">
       <c r="A35" s="7"/>
@@ -2109,7 +2171,9 @@
       <c r="C35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10">
+        <v>32</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="14.1" customHeight="1">
       <c r="A36" s="7"/>
@@ -2119,7 +2183,9 @@
       <c r="C36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="10">
+        <v>33</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="14.1" customHeight="1">
       <c r="A37" s="7"/>
@@ -2129,7 +2195,9 @@
       <c r="C37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="10"/>
+      <c r="D37" s="10">
+        <v>34</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="14.1" customHeight="1">
       <c r="A38" s="7"/>
@@ -2139,7 +2207,9 @@
       <c r="C38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="10"/>
+      <c r="D38" s="10">
+        <v>35</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="14.1" customHeight="1">
       <c r="A39" s="7"/>
@@ -2149,7 +2219,9 @@
       <c r="C39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="10"/>
+      <c r="D39" s="10">
+        <v>36</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="14.1" customHeight="1">
       <c r="A40" s="7"/>
@@ -2159,7 +2231,9 @@
       <c r="C40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="10">
+        <v>37</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="14.1" customHeight="1">
       <c r="A41" s="7"/>
@@ -2169,7 +2243,9 @@
       <c r="C41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="10">
+        <v>38</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="14.1" customHeight="1">
       <c r="A42" s="7"/>
@@ -2179,173 +2255,247 @@
       <c r="C42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="10">
+        <v>39</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="10"/>
+      <c r="D43" s="10">
+        <v>40</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="10">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="10"/>
+      <c r="D45" s="10">
+        <v>42</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="10">
+        <v>43</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10">
+        <v>44</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="2:3">
+      <c r="D48" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
       <c r="B49" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="2:3">
+      <c r="D49" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
       <c r="B50" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="2:3">
+      <c r="D50" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
       <c r="B51" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="52" spans="2:3">
+      <c r="D51" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
       <c r="B52" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="53" spans="2:3">
+      <c r="D52" s="10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
       <c r="B53" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="2:3">
+      <c r="D53" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
       <c r="B54" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="55" spans="2:3">
+      <c r="D54" s="10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
       <c r="B55" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="56" spans="2:3">
+      <c r="D55" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="57" spans="2:3">
+      <c r="D56" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
       <c r="B57" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="2:3">
+      <c r="D57" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
       <c r="B58" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="2:3">
+      <c r="D58" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
       <c r="B59" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="2:3">
+      <c r="D59" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
       <c r="B60" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="2:3">
+      <c r="D60" s="10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
       <c r="B61" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" ht="39.6">
+      <c r="D61" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="38.25">
       <c r="B62" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="2:3" ht="26.4">
+      <c r="D62" s="10">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="25.5">
       <c r="B63" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="2:3" ht="26.4">
+      <c r="D63" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="25.5">
       <c r="B64" s="11" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="2:108" ht="26.4">
+      <c r="D64" s="10">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:108" ht="25.5">
       <c r="B65" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="2:108" ht="39.6">
+      <c r="D65" s="10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="2:108" ht="38.25">
       <c r="B66" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="2:108" ht="66">
+      <c r="D66" s="10">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="2:108" ht="63.75">
       <c r="B67" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C67" s="2"/>
+      <c r="D67" s="10">
+        <v>64</v>
+      </c>
     </row>
     <row r="68" spans="2:108">
       <c r="B68" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D68" s="11"/>
+      <c r="D68" s="10">
+        <v>65</v>
+      </c>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -2440,7 +2590,9 @@
       <c r="B69" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="11"/>
+      <c r="D69" s="10">
+        <v>66</v>
+      </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
@@ -2538,7 +2690,9 @@
       <c r="B70" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D70" s="11"/>
+      <c r="D70" s="10">
+        <v>67</v>
+      </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
@@ -2638,7 +2792,9 @@
       <c r="B71" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="11"/>
+      <c r="D71" s="10">
+        <v>68</v>
+      </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2741,7 +2897,9 @@
       <c r="B72" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D72" s="11"/>
+      <c r="D72" s="10">
+        <v>69</v>
+      </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2847,7 +3005,9 @@
         <v>121</v>
       </c>
       <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
+      <c r="D73" s="10">
+        <v>70</v>
+      </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -2948,12 +3108,14 @@
       <c r="DC73" s="1"/>
       <c r="DD73" s="1"/>
     </row>
-    <row r="74" spans="2:108" ht="26.4">
+    <row r="74" spans="2:108" ht="25.5">
       <c r="B74" s="11" t="s">
         <v>80</v>
       </c>
       <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+      <c r="D74" s="10">
+        <v>71</v>
+      </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -3057,264 +3219,420 @@
       <c r="DC74" s="1"/>
       <c r="DD74" s="1"/>
     </row>
-    <row r="75" spans="2:108" ht="26.4">
+    <row r="75" spans="2:108" ht="25.5">
       <c r="B75" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="76" spans="2:108" ht="26.4">
+      <c r="D75" s="10">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="2:108" ht="25.5">
       <c r="B76" s="11" t="s">
         <v>106</v>
+      </c>
+      <c r="D76" s="10">
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="2:108">
       <c r="B77" s="11" t="s">
         <v>81</v>
       </c>
+      <c r="D77" s="10">
+        <v>74</v>
+      </c>
     </row>
     <row r="78" spans="2:108">
       <c r="B78" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="79" spans="2:108" ht="26.4">
+      <c r="D78" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="2:108" ht="25.5">
       <c r="B79" s="11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="80" spans="2:108" ht="26.4">
+      <c r="D79" s="10">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="2:108" ht="25.5">
       <c r="B80" s="11" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="81" spans="2:2">
+      <c r="D80" s="10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
       <c r="B81" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="82" spans="2:2">
+      <c r="D81" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
       <c r="B82" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="2:2">
+      <c r="D82" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
       <c r="B83" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="84" spans="2:2" ht="26.4">
+      <c r="D83" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="25.5">
       <c r="B84" s="11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" ht="26.4">
+      <c r="D84" s="10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" ht="25.5">
       <c r="B85" s="11" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" ht="26.4">
+      <c r="D85" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" ht="25.5">
       <c r="B86" s="11" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" ht="26.4">
+      <c r="D86" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" ht="25.5">
       <c r="B87" s="11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="88" spans="2:2">
+      <c r="D87" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
       <c r="B88" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="89" spans="2:2">
+      <c r="D88" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
       <c r="B89" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="90" spans="2:2" ht="26.4">
+      <c r="D89" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" ht="25.5">
       <c r="B90" s="11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="91" spans="2:2" ht="26.4">
+      <c r="D90" s="10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" ht="25.5">
       <c r="B91" s="11" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="92" spans="2:2" ht="26.4">
+      <c r="D91" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" ht="25.5">
       <c r="B92" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="93" spans="2:2" ht="26.4">
+      <c r="D92" s="10">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" ht="25.5">
       <c r="B93" s="11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="94" spans="2:2">
+      <c r="D93" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
       <c r="B94" s="11" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="95" spans="2:2" ht="26.4">
+      <c r="D94" s="10">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="25.5">
       <c r="B95" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="96" spans="2:2" ht="26.4">
+      <c r="D95" s="10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="25.5">
       <c r="B96" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" ht="26.4">
+      <c r="D96" s="10">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" ht="25.5">
       <c r="B97" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" ht="26.4">
+      <c r="D97" s="10">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" ht="25.5">
       <c r="B98" s="11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="99" spans="2:2" ht="39.6">
+      <c r="D98" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" ht="38.25">
       <c r="B99" s="11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="100" spans="2:2" ht="39.6">
+      <c r="D99" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" ht="38.25">
       <c r="B100" s="11" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="101" spans="2:2" ht="26.4">
+      <c r="D100" s="10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" ht="25.5">
       <c r="B101" s="11" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="102" spans="2:2" ht="26.4">
+      <c r="D101" s="10">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" ht="25.5">
       <c r="B102" s="11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="103" spans="2:2">
+      <c r="D102" s="10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4">
       <c r="B103" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="104" spans="2:2">
+      <c r="D103" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4">
       <c r="B104" s="11" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="105" spans="2:2">
+      <c r="D104" s="10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4">
       <c r="B105" s="11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="106" spans="2:2" ht="26.4">
+      <c r="D105" s="10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" ht="25.5">
       <c r="B106" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="107" spans="2:2">
+      <c r="D106" s="10">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4">
       <c r="B107" s="11" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="108" spans="2:2">
+      <c r="D107" s="10">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4">
       <c r="B108" s="11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="109" spans="2:2" ht="26.4">
+      <c r="D108" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" ht="25.5">
       <c r="B109" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="110" spans="2:2">
+      <c r="D109" s="10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4">
       <c r="B110" s="11" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="111" spans="2:2">
+      <c r="D110" s="10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4">
       <c r="B111" s="11" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="112" spans="2:2" ht="39.6">
+      <c r="D111" s="10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" ht="38.25">
       <c r="B112" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" ht="39.6">
+      <c r="D112" s="10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" ht="38.25">
       <c r="B113" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" ht="26.4">
+      <c r="D113" s="10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" ht="25.5">
       <c r="B114" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" ht="26.4">
+      <c r="D114" s="10">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" ht="25.5">
       <c r="B115" s="11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="116" spans="2:2">
+      <c r="D115" s="10">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4">
       <c r="B116" s="11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="117" spans="2:2">
+      <c r="D116" s="10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4">
       <c r="B117" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="118" spans="2:2">
+      <c r="D117" s="10">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4">
       <c r="B118" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="119" spans="2:2">
+      <c r="D118" s="10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4">
       <c r="B119" s="11" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="120" spans="2:2">
+      <c r="D119" s="10">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4">
       <c r="B120" s="11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="121" spans="2:2">
+      <c r="D120" s="10">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4">
       <c r="B121" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="122" spans="2:2">
+      <c r="D121" s="10">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4">
       <c r="B122" s="11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="123" spans="2:2">
+      <c r="D122" s="10">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4">
       <c r="B123" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" ht="26.4">
+      <c r="D123" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" ht="25.5">
       <c r="B124" s="11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" ht="26.4">
+      <c r="D124" s="10">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" ht="25.5">
       <c r="B125" s="11" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" ht="26.4">
+      <c r="D125" s="10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" ht="25.5">
       <c r="B126" s="11" t="s">
         <v>131</v>
+      </c>
+      <c r="D126" s="10">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>